<commit_message>
Correcciones 1 - Analisis espectral
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -1,42 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaqo\Desktop\facultad\materias\Señales y Sistemas\practicas\tp2\TP2_Varela_Muia_Dimitroff_Joaquín_Pablo_Juan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EDFA36-271E-494D-AE57-7117068AE84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibracion" sheetId="1" r:id="rId1"/>
     <sheet name="PR - SG" sheetId="2" r:id="rId2"/>
     <sheet name="RR - F1 - SG" sheetId="3" r:id="rId3"/>
-    <sheet name="SS 30 - 8K - F1 - SG" sheetId="4" r:id="rId4"/>
-    <sheet name="SS 70 - 6K - F1 - SG" sheetId="5" r:id="rId5"/>
-    <sheet name="SS 30 - 8K - F2 - SG" sheetId="7" r:id="rId6"/>
-    <sheet name="SS 30 - 8K - F1 - CG" sheetId="8" r:id="rId7"/>
-    <sheet name="SS 30 - 8K - F2 - CG" sheetId="9" r:id="rId8"/>
-    <sheet name="Signals - rir" sheetId="6" r:id="rId9"/>
+    <sheet name="RR - F2 - SG" sheetId="10" r:id="rId4"/>
+    <sheet name="SS 30 - 8K - F1 - SG" sheetId="4" r:id="rId5"/>
+    <sheet name="SS 70 - 6K - F1 - SG" sheetId="5" r:id="rId6"/>
+    <sheet name="SS 30 - 8K - F2 - SG" sheetId="7" r:id="rId7"/>
+    <sheet name="SS 30 - 8K - F1 - CG" sheetId="8" r:id="rId8"/>
+    <sheet name="SS 30 - 8K - F2 - CG" sheetId="9" r:id="rId9"/>
+    <sheet name="Signals - rir" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="117">
   <si>
     <t>Path</t>
   </si>
@@ -119,9 +117,6 @@
     <t>M1 - RR - F1 - SG</t>
   </si>
   <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/RR/Fuente 1/M1 - RR - F1 - SG.wav</t>
-  </si>
-  <si>
     <t>M2 - RR - F1 - SG</t>
   </si>
   <si>
@@ -137,21 +132,6 @@
     <t>M6 - RR - F1 - SG</t>
   </si>
   <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/RR/Fuente 1/M2 - RR - F1 - SG.wav</t>
-  </si>
-  <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/RR/Fuente 1/M3 - RR - F1 - SG.wav</t>
-  </si>
-  <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/RR/Fuente 1/M4 - RR - F1 - SG.wav</t>
-  </si>
-  <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/RR/Fuente 1/M5 - RR - F1 - SG.wav</t>
-  </si>
-  <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/RR/Fuente 1/M6 - RR - F1 - SG.wav</t>
-  </si>
-  <si>
     <t>M1 - SS 70 - 6K - F1 - SG</t>
   </si>
   <si>
@@ -351,13 +331,67 @@
   </si>
   <si>
     <t>./audios/3 - CASO 2 - AULA CON ESTUDIANTES/4 - BARRIDO LOGARITMICO 30Hz-8KHz/MEDICION 3/MIC 6 - Behringer ecm 8000_20.wav</t>
+  </si>
+  <si>
+    <t>M1 - RR - F2 - SG</t>
+  </si>
+  <si>
+    <t>M2 - RR - F2 - SG</t>
+  </si>
+  <si>
+    <t>M3 - RR - F2 - SG</t>
+  </si>
+  <si>
+    <t>M4 - RR - F2 - SG</t>
+  </si>
+  <si>
+    <t>M5 - RR - F2 - SG</t>
+  </si>
+  <si>
+    <t>M6 - RR - F2 - SG</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 1/MIC 1 - Earthworks M30_11.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 1/MIC 2 - Earthworks M30_11.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 1/MIC 3 - Behringer ecm 8000_13.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 1/MIC 4 - Behringer ecm 8000_12.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 1/MIC 5 - Behringer ecm 8000_12.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 1/MIC 6 - Behringer ecm 8000_12.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 2/MIC 1 - Earthworks M30_12.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 2/MIC 2 - Earthworks M30_12.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 2/MIC 3 - Behringer ecm 8000_14.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 2/MIC 4 - Behringer ecm 8000_13.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 2/MIC 5 - Behringer ecm 8000_13.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 2/MIC 6 - Behringer ecm 8000_13.wav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,27 +728,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="133.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -722,52 +756,175 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -776,20 +933,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -797,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -805,7 +962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -813,7 +970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -821,7 +978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -829,7 +986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -837,7 +994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -852,20 +1009,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="86.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -873,52 +1030,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -928,20 +1085,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2321DE76-FC56-4C80-8A28-BD52B08EF262}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="86.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -949,52 +1106,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1004,20 +1161,96 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="101.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="129.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1025,52 +1258,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1078,21 +1311,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="96.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1100,52 +1333,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1153,21 +1386,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="114.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1175,52 +1408,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1228,21 +1461,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="112.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1250,175 +1483,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="72.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parte 3 terminada, faltan corregir graficos subplot
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaqo\Desktop\facultad\materias\Señales y Sistemas\practicas\tp2\TP2_Varela_Muia_Dimitroff_Joaquín_Pablo_Juan\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EDFA36-271E-494D-AE57-7117068AE84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Calibracion" sheetId="1" r:id="rId1"/>
@@ -25,8 +19,8 @@
     <sheet name="Signals - rir" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -42,24 +36,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/PR/M1 - PR - SG.wav</t>
-  </si>
-  <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/PR/M2 - PR - SG.wav</t>
-  </si>
-  <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/PR/M3 - PR - SG.wav</t>
-  </si>
-  <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/PR/M4 - PR - SG.wav</t>
-  </si>
-  <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/PR/M5 - PR - SG.wav</t>
-  </si>
-  <si>
-    <t>./Mediciones Taller de Electrónica/Audios de Grabaciones/Sin Gente/PR/M6 - PR - SG.wav</t>
-  </si>
-  <si>
     <t>M1 - PR - SG</t>
   </si>
   <si>
@@ -385,13 +361,31 @@
   </si>
   <si>
     <t>./audios/2 - CASO 1 - AULA VACIA/1 - RUIDO ROSA/MEDICION 2/MIC 6 - Behringer ecm 8000_13.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/2 - PISO DE RUIDO/MIC 1 - Earthworks M30_03.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/2 - PISO DE RUIDO/MIC 2 - Earthworks M30_03.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/2 - PISO DE RUIDO/MIC 3 - Behringer ecm 8000_05.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/2 - PISO DE RUIDO/MIC 4 - Behringer ecm 8000_04.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/2 - PISO DE RUIDO/MIC 5 - Behringer ecm 8000_04.wav</t>
+  </si>
+  <si>
+    <t>./audios/2 - CASO 1 - AULA VACIA/2 - PISO DE RUIDO/MIC 6 - Behringer ecm 8000_04.wav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,27 +722,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="133.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -756,52 +750,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -810,20 +804,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.5703125" customWidth="1"/>
     <col min="2" max="2" width="72.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -831,100 +825,100 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B13" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -933,20 +927,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -954,52 +948,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1009,20 +1003,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="86.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1030,52 +1024,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1085,20 +1079,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2321DE76-FC56-4C80-8A28-BD52B08EF262}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="86.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1106,52 +1100,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1161,20 +1155,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="101.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1182,52 +1176,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1237,170 +1231,170 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="129.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="112" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="129.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="96.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="114.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1408,52 +1402,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1462,20 +1456,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="112.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1483,52 +1477,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>